<commit_message>
cut out rest opt
</commit_message>
<xml_diff>
--- a/metrics_comparison.xlsx
+++ b/metrics_comparison.xlsx
@@ -439,7 +439,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>20.08</v>
+        <v>18.76</v>
       </c>
       <c r="C3">
         <v>10.5</v>
@@ -461,7 +461,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>17.98</v>
+        <v>16.9</v>
       </c>
       <c r="C5">
         <v>14.52</v>
@@ -551,7 +551,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>13.57421875</v>
+        <v>9.3271484375</v>
       </c>
       <c r="C3">
         <v>0.7607421875</v>
@@ -573,7 +573,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3.9189453125</v>
+        <v>1.1728515625</v>
       </c>
       <c r="C5">
         <v>0.9482421875</v>

</xml_diff>

<commit_message>
results with final uc3
</commit_message>
<xml_diff>
--- a/metrics_comparison.xlsx
+++ b/metrics_comparison.xlsx
@@ -450,7 +450,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>16.7</v>
+        <v>15.16</v>
       </c>
       <c r="C4">
         <v>10.16</v>
@@ -562,7 +562,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>12.146484375</v>
+        <v>3.4765625</v>
       </c>
       <c r="C4">
         <v>1.7451171875</v>

</xml_diff>